<commit_message>
Adding code for new call functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData - Copy.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData - Copy.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E2058C79-198B-4E16-980A-57DDDB2C8212}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Companies" sheetId="2" r:id="rId2"/>
     <sheet name="Deals" sheetId="3" r:id="rId3"/>
+    <sheet name="Cases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="90">
   <si>
     <t>title</t>
   </si>
@@ -252,12 +251,48 @@
   </si>
   <si>
     <t>5000</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>CaseTitle1</t>
+  </si>
+  <si>
+    <t>CaseTitle2</t>
+  </si>
+  <si>
+    <t>Awaiting input</t>
+  </si>
+  <si>
+    <t>Enquiring</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>Business Support</t>
+  </si>
+  <si>
+    <t>Complaint</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>zzzx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,26 +425,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,23 +460,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -634,7 +635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -705,11 +706,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,11 +869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,4 +979,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding code for create new document functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData - Copy.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData - Copy.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="3"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Companies" sheetId="2" r:id="rId2"/>
     <sheet name="Deals" sheetId="3" r:id="rId3"/>
     <sheet name="Cases" sheetId="4" r:id="rId4"/>
+    <sheet name="Calls" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
   <si>
     <t>title</t>
   </si>
@@ -287,6 +288,36 @@
   </si>
   <si>
     <t>zzzx</t>
+  </si>
+  <si>
+    <t>deal</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>cccc</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>eeee</t>
+  </si>
+  <si>
+    <t>ffff</t>
+  </si>
+  <si>
+    <t>gggg</t>
+  </si>
+  <si>
+    <t>hhhh</t>
   </si>
 </sst>
 </file>
@@ -985,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,4 +1093,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>